<commit_message>
Some detailes have changed
</commit_message>
<xml_diff>
--- a/Numerical Experiments/Charts.xlsx
+++ b/Numerical Experiments/Charts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarzaminDigital\Desktop\PAPER\MATLAB\Numerical Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99DB88B-F573-4F69-A68A-0C7644529D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C14EC77-6B25-4754-95F8-3A1B0486519C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D6129A20-1F81-494B-BF6B-C0ED5DF90618}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
   <si>
     <t>NSGA-II</t>
   </si>
@@ -34,6 +34,21 @@
   </si>
   <si>
     <t>MOEA/D</t>
+  </si>
+  <si>
+    <t>MID</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>NPS</t>
+  </si>
+  <si>
+    <t>SNS</t>
+  </si>
+  <si>
+    <t>RAS</t>
   </si>
 </sst>
 </file>
@@ -77,13 +92,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1857,10 +1875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA82E70-FE4C-4668-AB26-ACA18349451D}">
-  <dimension ref="A2:AH27"/>
+  <dimension ref="A1:AK27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:V26"/>
+      <selection activeCell="AI1" sqref="AI1:AK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,12 +1896,51 @@
     <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="2.28515625" customWidth="1"/>
+    <col min="24" max="24" width="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="2" customWidth="1"/>
+    <col min="29" max="29" width="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="2.7109375" customWidth="1"/>
+    <col min="34" max="34" width="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="O1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="T1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="Y1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AD1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AI1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3"/>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="O2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1903,8 +1960,36 @@
       <c r="V2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="W2" s="2"/>
+      <c r="Y2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1939,34 +2024,43 @@
         <v>1.21</v>
       </c>
       <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
         <v>42.65</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>10.77</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>41.54</v>
       </c>
-      <c r="AB3">
-        <v>0.28999999999999998</v>
-      </c>
       <c r="AC3">
-        <v>0.17</v>
+        <v>1</v>
       </c>
       <c r="AD3">
         <v>0.28999999999999998</v>
       </c>
+      <c r="AE3">
+        <v>0.17</v>
+      </c>
       <c r="AF3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
         <v>0.56999999999999995</v>
       </c>
-      <c r="AG3">
+      <c r="AJ3">
         <v>0.11</v>
       </c>
-      <c r="AH3">
+      <c r="AK3">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -2004,34 +2098,43 @@
         <v>1.19</v>
       </c>
       <c r="X4">
+        <v>2</v>
+      </c>
+      <c r="Y4">
         <v>20.39</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>43.89</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>23.47</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
+        <v>2</v>
+      </c>
+      <c r="AD4">
         <v>0.12</v>
       </c>
-      <c r="AC4">
+      <c r="AE4">
         <v>0.23</v>
       </c>
-      <c r="AD4">
+      <c r="AF4">
         <v>0.15</v>
       </c>
-      <c r="AF4">
+      <c r="AH4">
+        <v>2</v>
+      </c>
+      <c r="AI4">
         <v>0.5</v>
       </c>
-      <c r="AG4">
+      <c r="AJ4">
         <v>0.8</v>
       </c>
-      <c r="AH4">
+      <c r="AK4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -2069,34 +2172,43 @@
         <v>0.92</v>
       </c>
       <c r="X5">
+        <v>3</v>
+      </c>
+      <c r="Y5">
         <v>27.35</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>34.4</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>36.729999999999997</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
+        <v>3</v>
+      </c>
+      <c r="AD5">
         <v>0.35</v>
       </c>
-      <c r="AC5">
+      <c r="AE5">
         <v>0.21</v>
       </c>
-      <c r="AD5">
+      <c r="AF5">
         <v>0.34</v>
       </c>
-      <c r="AF5">
+      <c r="AH5">
+        <v>3</v>
+      </c>
+      <c r="AI5">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AG5">
+      <c r="AJ5">
         <v>0.37</v>
       </c>
-      <c r="AH5">
+      <c r="AK5">
         <v>0.35</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -2134,34 +2246,43 @@
         <v>1.04</v>
       </c>
       <c r="X6">
+        <v>4</v>
+      </c>
+      <c r="Y6">
         <v>18.95</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>51.32</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <v>37.1</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
+        <v>4</v>
+      </c>
+      <c r="AD6">
         <v>0.21</v>
       </c>
-      <c r="AC6">
+      <c r="AE6">
         <v>0.1</v>
       </c>
-      <c r="AD6">
+      <c r="AF6">
         <v>0.22</v>
       </c>
-      <c r="AF6">
+      <c r="AH6">
+        <v>4</v>
+      </c>
+      <c r="AI6">
         <v>0.25</v>
       </c>
-      <c r="AG6">
+      <c r="AJ6">
         <v>0.44</v>
       </c>
-      <c r="AH6">
+      <c r="AK6">
         <v>0.48</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -2199,34 +2320,43 @@
         <v>1.01</v>
       </c>
       <c r="X7">
+        <v>5</v>
+      </c>
+      <c r="Y7">
         <v>39.49</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>83.99</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <v>51.78</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
+        <v>5</v>
+      </c>
+      <c r="AD7">
         <v>0.27</v>
       </c>
-      <c r="AC7">
+      <c r="AE7">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AD7">
+      <c r="AF7">
         <v>0.3</v>
       </c>
-      <c r="AF7">
+      <c r="AH7">
+        <v>5</v>
+      </c>
+      <c r="AI7">
         <v>0.5</v>
       </c>
-      <c r="AG7">
+      <c r="AJ7">
         <v>0.93</v>
       </c>
-      <c r="AH7">
+      <c r="AK7">
         <v>0.68</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -2264,34 +2394,43 @@
         <v>1.01</v>
       </c>
       <c r="X8">
+        <v>6</v>
+      </c>
+      <c r="Y8">
         <v>95.59</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>41.36</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <v>95.53</v>
       </c>
-      <c r="AB8">
+      <c r="AC8">
+        <v>6</v>
+      </c>
+      <c r="AD8">
         <v>0.22</v>
       </c>
-      <c r="AC8">
+      <c r="AE8">
         <v>0.13</v>
       </c>
-      <c r="AD8">
+      <c r="AF8">
         <v>0.23</v>
       </c>
-      <c r="AF8">
+      <c r="AH8">
+        <v>6</v>
+      </c>
+      <c r="AI8">
         <v>0.69</v>
       </c>
-      <c r="AG8">
+      <c r="AJ8">
         <v>0.41</v>
       </c>
-      <c r="AH8">
+      <c r="AK8">
         <v>0.7</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -2329,34 +2468,43 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="X9">
+        <v>7</v>
+      </c>
+      <c r="Y9">
         <v>67.16</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>79.569999999999993</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <v>75.31</v>
       </c>
-      <c r="AB9">
+      <c r="AC9">
+        <v>7</v>
+      </c>
+      <c r="AD9">
         <v>0.15</v>
       </c>
-      <c r="AC9">
+      <c r="AE9">
         <v>0.13</v>
       </c>
-      <c r="AD9">
+      <c r="AF9">
         <v>0.18</v>
       </c>
-      <c r="AF9">
+      <c r="AH9">
+        <v>7</v>
+      </c>
+      <c r="AI9">
         <v>0.56000000000000005</v>
       </c>
-      <c r="AG9">
+      <c r="AJ9">
         <v>0.74</v>
       </c>
-      <c r="AH9">
+      <c r="AK9">
         <v>0.65</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -2394,34 +2542,43 @@
         <v>1.21</v>
       </c>
       <c r="X10">
+        <v>8</v>
+      </c>
+      <c r="Y10">
         <v>15.31</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>16.670000000000002</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <v>12.66</v>
       </c>
-      <c r="AB10">
-        <v>0.28999999999999998</v>
-      </c>
       <c r="AC10">
-        <v>0.17</v>
+        <v>8</v>
       </c>
       <c r="AD10">
         <v>0.28999999999999998</v>
       </c>
+      <c r="AE10">
+        <v>0.17</v>
+      </c>
       <c r="AF10">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AH10">
+        <v>8</v>
+      </c>
+      <c r="AI10">
         <v>0.21</v>
       </c>
-      <c r="AG10">
+      <c r="AJ10">
         <v>0.12</v>
       </c>
-      <c r="AH10">
+      <c r="AK10">
         <v>0.19</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -2459,34 +2616,43 @@
         <v>0.98</v>
       </c>
       <c r="X11">
+        <v>9</v>
+      </c>
+      <c r="Y11">
         <v>30.23</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>55.48</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <v>40</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
+        <v>9</v>
+      </c>
+      <c r="AD11">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AC11">
+      <c r="AE11">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AD11">
+      <c r="AF11">
         <v>0.32</v>
       </c>
-      <c r="AF11">
+      <c r="AH11">
+        <v>9</v>
+      </c>
+      <c r="AI11">
         <v>0.37</v>
       </c>
-      <c r="AG11">
+      <c r="AJ11">
         <v>0.27</v>
       </c>
-      <c r="AH11">
+      <c r="AK11">
         <v>0.23</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -2524,34 +2690,43 @@
         <v>1.02</v>
       </c>
       <c r="X12">
+        <v>10</v>
+      </c>
+      <c r="Y12">
         <v>55.54</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <v>70.91</v>
       </c>
-      <c r="Z12">
+      <c r="AA12">
         <v>60.38</v>
       </c>
-      <c r="AB12">
+      <c r="AC12">
+        <v>10</v>
+      </c>
+      <c r="AD12">
         <v>0.32</v>
       </c>
-      <c r="AC12">
+      <c r="AE12">
         <v>0.26</v>
       </c>
-      <c r="AD12">
+      <c r="AF12">
         <v>0.31</v>
       </c>
-      <c r="AF12">
+      <c r="AH12">
+        <v>10</v>
+      </c>
+      <c r="AI12">
         <v>0.47</v>
       </c>
-      <c r="AG12">
+      <c r="AJ12">
         <v>0.78</v>
       </c>
-      <c r="AH12">
+      <c r="AK12">
         <v>0.81</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -2589,34 +2764,43 @@
         <v>1.01</v>
       </c>
       <c r="X13">
+        <v>11</v>
+      </c>
+      <c r="Y13">
         <v>221.4</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>60.23</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>65.53</v>
       </c>
-      <c r="AB13">
+      <c r="AC13">
+        <v>11</v>
+      </c>
+      <c r="AD13">
         <v>0.19</v>
       </c>
-      <c r="AC13">
+      <c r="AE13">
         <v>0.24</v>
       </c>
-      <c r="AD13">
+      <c r="AF13">
         <v>0.21</v>
       </c>
-      <c r="AF13">
+      <c r="AH13">
+        <v>11</v>
+      </c>
+      <c r="AI13">
         <v>1.06</v>
       </c>
-      <c r="AG13">
+      <c r="AJ13">
         <v>0.34</v>
       </c>
-      <c r="AH13">
+      <c r="AK13">
         <v>0.34</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -2654,34 +2838,43 @@
         <v>1.01</v>
       </c>
       <c r="X14">
+        <v>12</v>
+      </c>
+      <c r="Y14">
         <v>62.92</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <v>104</v>
       </c>
-      <c r="Z14">
+      <c r="AA14">
         <v>74.290000000000006</v>
       </c>
-      <c r="AB14">
+      <c r="AC14">
+        <v>12</v>
+      </c>
+      <c r="AD14">
         <v>0.15</v>
       </c>
-      <c r="AC14">
+      <c r="AE14">
         <v>0.13</v>
       </c>
-      <c r="AD14">
+      <c r="AF14">
         <v>0.23</v>
       </c>
-      <c r="AF14">
+      <c r="AH14">
+        <v>12</v>
+      </c>
+      <c r="AI14">
         <v>0.42</v>
       </c>
-      <c r="AG14">
+      <c r="AJ14">
         <v>0.49</v>
       </c>
-      <c r="AH14">
+      <c r="AK14">
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -2719,34 +2912,43 @@
         <v>0.94</v>
       </c>
       <c r="X15">
+        <v>13</v>
+      </c>
+      <c r="Y15">
         <v>193.1</v>
       </c>
-      <c r="Y15">
+      <c r="Z15">
         <v>217.4</v>
       </c>
-      <c r="Z15">
+      <c r="AA15">
         <v>202.3</v>
       </c>
-      <c r="AB15">
+      <c r="AC15">
+        <v>13</v>
+      </c>
+      <c r="AD15">
         <v>0.24</v>
       </c>
-      <c r="AC15">
+      <c r="AE15">
         <v>0.11</v>
       </c>
-      <c r="AD15">
+      <c r="AF15">
         <v>0.39</v>
       </c>
-      <c r="AF15">
+      <c r="AH15">
+        <v>13</v>
+      </c>
+      <c r="AI15">
         <v>0.37</v>
       </c>
-      <c r="AG15">
+      <c r="AJ15">
         <v>0.48</v>
       </c>
-      <c r="AH15">
+      <c r="AK15">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -2784,34 +2986,43 @@
         <v>0.87</v>
       </c>
       <c r="X16">
+        <v>14</v>
+      </c>
+      <c r="Y16">
         <v>313.89999999999998</v>
       </c>
-      <c r="Y16">
+      <c r="Z16">
         <v>341.4</v>
       </c>
-      <c r="Z16">
+      <c r="AA16">
         <v>179.2</v>
       </c>
-      <c r="AB16">
+      <c r="AC16">
+        <v>14</v>
+      </c>
+      <c r="AD16">
         <v>0.18</v>
       </c>
-      <c r="AC16">
+      <c r="AE16">
         <v>0.13</v>
       </c>
-      <c r="AD16">
+      <c r="AF16">
         <v>0.33</v>
       </c>
-      <c r="AF16">
+      <c r="AH16">
+        <v>14</v>
+      </c>
+      <c r="AI16">
         <v>1.04</v>
       </c>
-      <c r="AG16">
+      <c r="AJ16">
         <v>0.99</v>
       </c>
-      <c r="AH16">
+      <c r="AK16">
         <v>0.48</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>14</v>
       </c>
@@ -2849,34 +3060,43 @@
         <v>0.93</v>
       </c>
       <c r="X17">
+        <v>15</v>
+      </c>
+      <c r="Y17">
         <v>118.2</v>
       </c>
-      <c r="Y17">
+      <c r="Z17">
         <v>254.4</v>
       </c>
-      <c r="Z17">
+      <c r="AA17">
         <v>277.8</v>
       </c>
-      <c r="AB17">
+      <c r="AC17">
+        <v>15</v>
+      </c>
+      <c r="AD17">
         <v>0.11</v>
       </c>
-      <c r="AC17">
+      <c r="AE17">
         <v>0.25</v>
       </c>
-      <c r="AD17">
+      <c r="AF17">
         <v>0.53</v>
       </c>
-      <c r="AF17">
+      <c r="AH17">
+        <v>15</v>
+      </c>
+      <c r="AI17">
         <v>0.18</v>
       </c>
-      <c r="AG17">
+      <c r="AJ17">
         <v>0.3</v>
       </c>
-      <c r="AH17">
+      <c r="AK17">
         <v>0.27</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -2914,34 +3134,43 @@
         <v>0.96</v>
       </c>
       <c r="X18">
+        <v>16</v>
+      </c>
+      <c r="Y18">
         <v>82.26</v>
       </c>
-      <c r="Y18">
+      <c r="Z18">
         <v>29.14</v>
       </c>
-      <c r="Z18">
+      <c r="AA18">
         <v>95.06</v>
       </c>
-      <c r="AB18">
-        <v>0.33</v>
-      </c>
       <c r="AC18">
-        <v>0.22</v>
+        <v>16</v>
       </c>
       <c r="AD18">
         <v>0.33</v>
       </c>
+      <c r="AE18">
+        <v>0.22</v>
+      </c>
       <c r="AF18">
+        <v>0.33</v>
+      </c>
+      <c r="AH18">
+        <v>16</v>
+      </c>
+      <c r="AI18">
         <v>0.16</v>
       </c>
-      <c r="AG18">
+      <c r="AJ18">
         <v>0.08</v>
       </c>
-      <c r="AH18">
+      <c r="AK18">
         <v>0.24</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -2979,34 +3208,43 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="X19">
+        <v>17</v>
+      </c>
+      <c r="Y19">
         <v>252.2</v>
       </c>
-      <c r="Y19">
+      <c r="Z19">
         <v>555.79999999999995</v>
       </c>
-      <c r="Z19">
+      <c r="AA19">
         <v>78.89</v>
       </c>
-      <c r="AB19">
-        <v>0.27</v>
-      </c>
       <c r="AC19">
-        <v>0.19</v>
+        <v>17</v>
       </c>
       <c r="AD19">
         <v>0.27</v>
       </c>
+      <c r="AE19">
+        <v>0.19</v>
+      </c>
       <c r="AF19">
+        <v>0.27</v>
+      </c>
+      <c r="AH19">
+        <v>17</v>
+      </c>
+      <c r="AI19">
         <v>0.63</v>
       </c>
-      <c r="AG19">
+      <c r="AJ19">
         <v>0.71</v>
       </c>
-      <c r="AH19">
+      <c r="AK19">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -3044,34 +3282,43 @@
         <v>1.06</v>
       </c>
       <c r="X20">
+        <v>18</v>
+      </c>
+      <c r="Y20">
         <v>185.2</v>
       </c>
-      <c r="Y20">
+      <c r="Z20">
         <v>117.6</v>
       </c>
-      <c r="Z20">
+      <c r="AA20">
         <v>89.38</v>
       </c>
-      <c r="AB20">
+      <c r="AC20">
+        <v>18</v>
+      </c>
+      <c r="AD20">
         <v>0.39</v>
       </c>
-      <c r="AC20">
+      <c r="AE20">
         <v>0.11</v>
       </c>
-      <c r="AD20">
+      <c r="AF20">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AF20">
+      <c r="AH20">
+        <v>18</v>
+      </c>
+      <c r="AI20">
         <v>0.24</v>
       </c>
-      <c r="AG20">
+      <c r="AJ20">
         <v>0.24</v>
       </c>
-      <c r="AH20">
+      <c r="AK20">
         <v>0.21</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -3109,34 +3356,43 @@
         <v>0.99</v>
       </c>
       <c r="X21">
+        <v>19</v>
+      </c>
+      <c r="Y21">
         <v>231.3</v>
       </c>
-      <c r="Y21">
+      <c r="Z21">
         <v>702.7</v>
       </c>
-      <c r="Z21">
+      <c r="AA21">
         <v>627.1</v>
       </c>
-      <c r="AB21">
+      <c r="AC21">
+        <v>19</v>
+      </c>
+      <c r="AD21">
         <v>0.36</v>
       </c>
-      <c r="AC21">
+      <c r="AE21">
         <v>0.16</v>
-      </c>
-      <c r="AD21">
-        <v>0.21</v>
       </c>
       <c r="AF21">
         <v>0.21</v>
       </c>
-      <c r="AG21">
+      <c r="AH21">
+        <v>19</v>
+      </c>
+      <c r="AI21">
+        <v>0.21</v>
+      </c>
+      <c r="AJ21">
         <v>1.02</v>
       </c>
-      <c r="AH21">
+      <c r="AK21">
         <v>0.43</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>19</v>
       </c>
@@ -3174,34 +3430,43 @@
         <v>1.18</v>
       </c>
       <c r="X22">
+        <v>20</v>
+      </c>
+      <c r="Y22">
         <v>235.3</v>
       </c>
-      <c r="Y22">
+      <c r="Z22">
         <v>400.1</v>
       </c>
-      <c r="Z22">
+      <c r="AA22">
         <v>277</v>
       </c>
-      <c r="AB22">
+      <c r="AC22">
+        <v>20</v>
+      </c>
+      <c r="AD22">
         <v>0.18</v>
       </c>
-      <c r="AC22">
+      <c r="AE22">
         <v>0.12</v>
       </c>
-      <c r="AD22">
+      <c r="AF22">
         <v>0.24</v>
       </c>
-      <c r="AF22">
+      <c r="AH22">
+        <v>20</v>
+      </c>
+      <c r="AI22">
         <v>0.3</v>
       </c>
-      <c r="AG22">
+      <c r="AJ22">
         <v>0.54</v>
       </c>
-      <c r="AH22">
+      <c r="AK22">
         <v>0.44</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>20</v>
       </c>
@@ -3239,34 +3504,43 @@
         <v>1.06</v>
       </c>
       <c r="X23">
+        <v>21</v>
+      </c>
+      <c r="Y23">
         <v>192.6</v>
       </c>
-      <c r="Y23">
+      <c r="Z23">
         <v>222.1</v>
       </c>
-      <c r="Z23">
+      <c r="AA23">
         <v>175.5</v>
       </c>
-      <c r="AB23">
+      <c r="AC23">
+        <v>21</v>
+      </c>
+      <c r="AD23">
         <v>0.18</v>
       </c>
-      <c r="AC23">
+      <c r="AE23">
         <v>0.11</v>
       </c>
-      <c r="AD23">
+      <c r="AF23">
         <v>0.17</v>
       </c>
-      <c r="AF23">
+      <c r="AH23">
+        <v>21</v>
+      </c>
+      <c r="AI23">
         <v>0.22</v>
       </c>
-      <c r="AG23">
+      <c r="AJ23">
         <v>0.22</v>
       </c>
-      <c r="AH23">
+      <c r="AK23">
         <v>0.18</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -3304,34 +3578,43 @@
         <v>0.85</v>
       </c>
       <c r="X24">
+        <v>22</v>
+      </c>
+      <c r="Y24">
         <v>214.6</v>
       </c>
-      <c r="Y24">
+      <c r="Z24">
         <v>254.5</v>
       </c>
-      <c r="Z24">
+      <c r="AA24">
         <v>192.6</v>
       </c>
-      <c r="AB24">
+      <c r="AC24">
+        <v>22</v>
+      </c>
+      <c r="AD24">
         <v>0.21</v>
       </c>
-      <c r="AC24">
+      <c r="AE24">
         <v>0.12</v>
       </c>
-      <c r="AD24">
+      <c r="AF24">
         <v>0.54</v>
       </c>
-      <c r="AF24">
+      <c r="AH24">
+        <v>22</v>
+      </c>
+      <c r="AI24">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AG24">
+      <c r="AJ24">
         <v>0.31</v>
       </c>
-      <c r="AH24">
+      <c r="AK24">
         <v>0.19</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -3369,34 +3652,43 @@
         <v>1.05</v>
       </c>
       <c r="X25">
+        <v>23</v>
+      </c>
+      <c r="Y25">
         <v>394.5</v>
       </c>
-      <c r="Y25">
+      <c r="Z25">
         <v>218.1</v>
       </c>
-      <c r="Z25">
+      <c r="AA25">
         <v>364.1</v>
       </c>
-      <c r="AB25">
+      <c r="AC25">
+        <v>23</v>
+      </c>
+      <c r="AD25">
         <v>0.21</v>
       </c>
-      <c r="AC25">
+      <c r="AE25">
         <v>0.17</v>
       </c>
-      <c r="AD25">
+      <c r="AF25">
         <v>0.18</v>
       </c>
-      <c r="AF25">
+      <c r="AH25">
+        <v>23</v>
+      </c>
+      <c r="AI25">
         <v>0.24</v>
       </c>
-      <c r="AG25">
+      <c r="AJ25">
         <v>0.12</v>
       </c>
-      <c r="AH25">
+      <c r="AK25">
         <v>0.3</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>23</v>
       </c>
@@ -3434,34 +3726,43 @@
         <v>0.78</v>
       </c>
       <c r="X26">
+        <v>24</v>
+      </c>
+      <c r="Y26">
         <v>205.8</v>
       </c>
-      <c r="Y26">
+      <c r="Z26">
         <v>408.3</v>
       </c>
-      <c r="Z26">
+      <c r="AA26">
         <v>436.5</v>
       </c>
-      <c r="AB26">
+      <c r="AC26">
+        <v>24</v>
+      </c>
+      <c r="AD26">
         <v>0.23</v>
       </c>
-      <c r="AC26">
+      <c r="AE26">
         <v>0.22</v>
       </c>
-      <c r="AD26">
+      <c r="AF26">
         <v>0.52</v>
       </c>
-      <c r="AF26">
+      <c r="AH26">
+        <v>24</v>
+      </c>
+      <c r="AI26">
         <v>0.15</v>
       </c>
-      <c r="AG26">
+      <c r="AJ26">
         <v>0.45</v>
       </c>
-      <c r="AH26">
+      <c r="AK26">
         <v>0.26</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>24</v>
       </c>
@@ -3476,6 +3777,13 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="AD1:AF1"/>
+    <mergeCell ref="AI1:AK1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Vikor finished + Entropy started
</commit_message>
<xml_diff>
--- a/Numerical Experiments/Charts.xlsx
+++ b/Numerical Experiments/Charts.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inosoft_04\Desktop\PAPER\MATLAB\Numerical Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B91CE6-74DE-40D9-9984-7408EC93FF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5349A29A-E369-462D-9FDA-7B66EEA5295B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{D6129A20-1F81-494B-BF6B-C0ED5DF90618}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Entropy" sheetId="3" r:id="rId2"/>
+    <sheet name="Vikor" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="25">
   <si>
     <t>NSGA-II</t>
   </si>
@@ -108,11 +109,17 @@
   <si>
     <t>→</t>
   </si>
+  <si>
+    <t>Sum</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,7 +194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -232,11 +239,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -246,9 +262,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -262,15 +275,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -281,9 +285,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -303,6 +304,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,48 +679,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="I1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="P1" s="4" t="s">
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="P1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="W1" s="4" t="s">
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="W1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AD1" s="4" t="s">
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AD1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AK1" s="4" t="s">
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="19"/>
+      <c r="AK1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AL1" s="4"/>
-      <c r="AM1" s="4"/>
-      <c r="AN1" s="4"/>
-      <c r="AO1" s="4"/>
+      <c r="AL1" s="19"/>
+      <c r="AM1" s="19"/>
+      <c r="AN1" s="19"/>
+      <c r="AO1" s="19"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -3815,12 +3837,987 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D37A0FC-DBA9-4B44-8E5C-722A81CC8EDB}">
+  <dimension ref="B3:P25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="2.5703125" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.1628212500000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>41.3352875</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.28368749999999993</v>
+      </c>
+      <c r="G4" s="1">
+        <v>9.1118625000000009</v>
+      </c>
+      <c r="H4" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="24">
+        <f>C4/$C$9</f>
+        <v>8.6493679308050561E-2</v>
+      </c>
+      <c r="L4" s="24">
+        <f>D4/$D$9</f>
+        <v>0.21382023375817408</v>
+      </c>
+      <c r="M4" s="24">
+        <f>E4/$E$9</f>
+        <v>0.19503727484500177</v>
+      </c>
+      <c r="N4" s="24">
+        <f>F4/$F$9</f>
+        <v>0.23463402984333948</v>
+      </c>
+      <c r="O4" s="24">
+        <f>G4/$G$9</f>
+        <v>0.19979733815146303</v>
+      </c>
+      <c r="P4" s="24">
+        <f>H4/$H$9</f>
+        <v>2.3366560582481623E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.0776162499999999</v>
+      </c>
+      <c r="E5" s="1">
+        <v>41.723300000000002</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.24895249999999997</v>
+      </c>
+      <c r="G5" s="1">
+        <v>9.4863999999999997</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.91874999999999996</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="24">
+        <f t="shared" ref="K5:K8" si="0">C5/$C$9</f>
+        <v>0.19161676646706585</v>
+      </c>
+      <c r="L5" s="24">
+        <f t="shared" ref="L5:L8" si="1">D5/$D$9</f>
+        <v>0.19815268982795672</v>
+      </c>
+      <c r="M5" s="24">
+        <f t="shared" ref="M5:M8" si="2">E5/$E$9</f>
+        <v>0.19686808104432474</v>
+      </c>
+      <c r="N5" s="24">
+        <f t="shared" ref="N5:N8" si="3">F5/$F$9</f>
+        <v>0.20590518903573116</v>
+      </c>
+      <c r="O5" s="24">
+        <f t="shared" ref="O5:O8" si="4">G5/$G$9</f>
+        <v>0.20800988476725132</v>
+      </c>
+      <c r="P5" s="24">
+        <f t="shared" ref="P5:P8" si="5">H5/$H$9</f>
+        <v>0.34348844056247985</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.25</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.0680375000000002</v>
+      </c>
+      <c r="E6" s="1">
+        <v>41.897987499999999</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.23678625000000003</v>
+      </c>
+      <c r="G6" s="1">
+        <v>9.5143249999999995</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.87467499999999998</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="24">
+        <f t="shared" si="0"/>
+        <v>0.21956087824351295</v>
+      </c>
+      <c r="L6" s="24">
+        <f t="shared" si="1"/>
+        <v>0.19639134382218751</v>
+      </c>
+      <c r="M6" s="24">
+        <f t="shared" si="2"/>
+        <v>0.19769233015471221</v>
+      </c>
+      <c r="N6" s="24">
+        <f t="shared" si="3"/>
+        <v>0.19584265097684059</v>
+      </c>
+      <c r="O6" s="24">
+        <f t="shared" si="4"/>
+        <v>0.20862220092850592</v>
+      </c>
+      <c r="P6" s="24">
+        <f t="shared" si="5"/>
+        <v>0.3270103420397138</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.0519937500000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>43.401162500000005</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.24605874999999999</v>
+      </c>
+      <c r="G7" s="1">
+        <v>9.5867374999999999</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.8188375</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="24">
+        <f t="shared" si="0"/>
+        <v>0.23952095808383231</v>
+      </c>
+      <c r="L7" s="24">
+        <f t="shared" si="1"/>
+        <v>0.19344120993414776</v>
+      </c>
+      <c r="M7" s="24">
+        <f t="shared" si="2"/>
+        <v>0.20478494214187057</v>
+      </c>
+      <c r="N7" s="24">
+        <f t="shared" si="3"/>
+        <v>0.20351180820697007</v>
+      </c>
+      <c r="O7" s="24">
+        <f t="shared" si="4"/>
+        <v>0.2102100019679633</v>
+      </c>
+      <c r="P7" s="24">
+        <f t="shared" si="5"/>
+        <v>0.30613465681532476</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9.875</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.07784375</v>
+      </c>
+      <c r="E8" s="1">
+        <v>43.577583750000002</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.19357875000000002</v>
+      </c>
+      <c r="G8" s="1">
+        <v>7.9062000000000001</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="24">
+        <f t="shared" si="0"/>
+        <v>0.26280771789753826</v>
+      </c>
+      <c r="L8" s="24">
+        <f t="shared" si="1"/>
+        <v>0.19819452265753393</v>
+      </c>
+      <c r="M8" s="24">
+        <f t="shared" si="2"/>
+        <v>0.20561737181409065</v>
+      </c>
+      <c r="N8" s="24">
+        <f t="shared" si="3"/>
+        <v>0.16010632193711874</v>
+      </c>
+      <c r="O8" s="24">
+        <f t="shared" si="4"/>
+        <v>0.17336057418481643</v>
+      </c>
+      <c r="P8" s="24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="25">
+        <f>SUM(C4:C8)</f>
+        <v>37.575000000000003</v>
+      </c>
+      <c r="D9" s="25">
+        <f t="shared" ref="D9:H9" si="6">SUM(D4:D8)</f>
+        <v>5.4383125000000003</v>
+      </c>
+      <c r="E9" s="25">
+        <f t="shared" si="6"/>
+        <v>211.93532125000002</v>
+      </c>
+      <c r="F9" s="25">
+        <f t="shared" si="6"/>
+        <v>1.2090637499999999</v>
+      </c>
+      <c r="G9" s="25">
+        <f t="shared" si="6"/>
+        <v>45.605525</v>
+      </c>
+      <c r="H9" s="25">
+        <f t="shared" si="6"/>
+        <v>2.6747624999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3.625</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.0283912499999999</v>
+      </c>
+      <c r="E12" s="1">
+        <v>105.5400125</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.36161624999999997</v>
+      </c>
+      <c r="G12" s="1">
+        <v>15.109075000000001</v>
+      </c>
+      <c r="H12" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="24">
+        <f>C12/$C$17</f>
+        <v>3.689567430025445E-2</v>
+      </c>
+      <c r="L12" s="24">
+        <f>D12/$D$17</f>
+        <v>0.21225650355827813</v>
+      </c>
+      <c r="M12" s="24">
+        <f>E12/$E$17</f>
+        <v>0.17641879131537064</v>
+      </c>
+      <c r="N12" s="24">
+        <f>F12/$F$17</f>
+        <v>0.3044371018570376</v>
+      </c>
+      <c r="O12" s="24">
+        <f>G12/$G$17</f>
+        <v>0.18672447941262843</v>
+      </c>
+      <c r="P12" s="24">
+        <f>H12/$H$17</f>
+        <v>3.5692105620078948E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>17.375</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.87214000000000003</v>
+      </c>
+      <c r="E13" s="1">
+        <v>124.864625</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.23612000000000002</v>
+      </c>
+      <c r="G13" s="1">
+        <v>16.849350000000001</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.49032500000000001</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="24">
+        <f t="shared" ref="K13:K16" si="7">C13/$C$17</f>
+        <v>0.17684478371501272</v>
+      </c>
+      <c r="L13" s="24">
+        <f t="shared" ref="L13:L16" si="8">D13/$D$17</f>
+        <v>0.18000676980994998</v>
+      </c>
+      <c r="M13" s="24">
+        <f t="shared" ref="M13:M16" si="9">E13/$E$17</f>
+        <v>0.20872146685170245</v>
+      </c>
+      <c r="N13" s="24">
+        <f t="shared" ref="N13:N16" si="10">F13/$F$17</f>
+        <v>0.19878445310597553</v>
+      </c>
+      <c r="O13" s="24">
+        <f t="shared" ref="O13:O16" si="11">G13/$G$17</f>
+        <v>0.20823155005790697</v>
+      </c>
+      <c r="P13" s="24">
+        <f t="shared" ref="P13:P16" si="12">H13/$H$17</f>
+        <v>0.28001170701064337</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>25.25</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.94584125000000008</v>
+      </c>
+      <c r="E14" s="1">
+        <v>104.21896249999999</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.20113624999999999</v>
+      </c>
+      <c r="G14" s="1">
+        <v>16.796424999999999</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.56166249999999995</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" s="24">
+        <f t="shared" si="7"/>
+        <v>0.25699745547073793</v>
+      </c>
+      <c r="L14" s="24">
+        <f t="shared" si="8"/>
+        <v>0.19521846052870567</v>
+      </c>
+      <c r="M14" s="24">
+        <f t="shared" si="9"/>
+        <v>0.17421054783740847</v>
+      </c>
+      <c r="N14" s="24">
+        <f t="shared" si="10"/>
+        <v>0.16933237106571558</v>
+      </c>
+      <c r="O14" s="24">
+        <f t="shared" si="11"/>
+        <v>0.2075774800322493</v>
+      </c>
+      <c r="P14" s="24">
+        <f t="shared" si="12"/>
+        <v>0.32075067636540144</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.92153000000000007</v>
+      </c>
+      <c r="E15" s="1">
+        <v>113.69499999999999</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.20208625000000002</v>
+      </c>
+      <c r="G15" s="1">
+        <v>16.938724999999998</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.63659999999999994</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="24">
+        <f t="shared" si="7"/>
+        <v>0.26463104325699743</v>
+      </c>
+      <c r="L15" s="24">
+        <f t="shared" si="8"/>
+        <v>0.19020070009741924</v>
+      </c>
+      <c r="M15" s="24">
+        <f t="shared" si="9"/>
+        <v>0.19005052210507425</v>
+      </c>
+      <c r="N15" s="24">
+        <f t="shared" si="10"/>
+        <v>0.17013215604983672</v>
+      </c>
+      <c r="O15" s="24">
+        <f t="shared" si="11"/>
+        <v>0.20933608493826883</v>
+      </c>
+      <c r="P15" s="24">
+        <f t="shared" si="12"/>
+        <v>0.36354551100387611</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.0771375000000001</v>
+      </c>
+      <c r="E16" s="1">
+        <v>149.91706249999999</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.18686049999999998</v>
+      </c>
+      <c r="G16" s="1">
+        <v>15.222837500000001</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="24">
+        <f t="shared" si="7"/>
+        <v>0.26463104325699743</v>
+      </c>
+      <c r="L16" s="24">
+        <f t="shared" si="8"/>
+        <v>0.22231756600564703</v>
+      </c>
+      <c r="M16" s="24">
+        <f t="shared" si="9"/>
+        <v>0.25059867189044416</v>
+      </c>
+      <c r="N16" s="24">
+        <f t="shared" si="10"/>
+        <v>0.15731391792143459</v>
+      </c>
+      <c r="O16" s="24">
+        <f t="shared" si="11"/>
+        <v>0.18813040555894639</v>
+      </c>
+      <c r="P16" s="24">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="25">
+        <f>SUM(C12:C16)</f>
+        <v>98.25</v>
+      </c>
+      <c r="D17" s="25">
+        <f t="shared" ref="D17:H17" si="13">SUM(D12:D16)</f>
+        <v>4.84504</v>
+      </c>
+      <c r="E17" s="25">
+        <f t="shared" si="13"/>
+        <v>598.23566249999999</v>
+      </c>
+      <c r="F17" s="25">
+        <f t="shared" si="13"/>
+        <v>1.18781925</v>
+      </c>
+      <c r="G17" s="25">
+        <f t="shared" si="13"/>
+        <v>80.916412500000007</v>
+      </c>
+      <c r="H17" s="25">
+        <f t="shared" si="13"/>
+        <v>1.7510875000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.06041125</v>
+      </c>
+      <c r="E20" s="1">
+        <v>137.13126249999999</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.33305875000000001</v>
+      </c>
+      <c r="G20" s="1">
+        <v>30.2416625</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="24">
+        <f>C20/$C$25</f>
+        <v>3.1668696711327646E-2</v>
+      </c>
+      <c r="L20" s="24">
+        <f>D20/$D$25</f>
+        <v>0.23041016931567287</v>
+      </c>
+      <c r="M20" s="24">
+        <f>E20/$E$25</f>
+        <v>0.12207820767374607</v>
+      </c>
+      <c r="N20" s="24">
+        <f>F20/$F$25</f>
+        <v>0.24999772470891993</v>
+      </c>
+      <c r="O20" s="24">
+        <f>G20/$G$25</f>
+        <v>0.1975009245101729</v>
+      </c>
+      <c r="P20" s="24">
+        <f>H20/$H$25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>17.75</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.77668875000000004</v>
+      </c>
+      <c r="E21" s="1">
+        <v>193.93778750000001</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.284055</v>
+      </c>
+      <c r="G21" s="1">
+        <v>31.714412500000002</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.43057499999999999</v>
+      </c>
+      <c r="J21" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" s="24">
+        <f t="shared" ref="K21:K24" si="14">C21/$C$25</f>
+        <v>0.17295980511571254</v>
+      </c>
+      <c r="L21" s="24">
+        <f t="shared" ref="L21:L24" si="15">D21/$D$25</f>
+        <v>0.16876187082424704</v>
+      </c>
+      <c r="M21" s="24">
+        <f t="shared" ref="M21:M24" si="16">E21/$E$25</f>
+        <v>0.17264901574294073</v>
+      </c>
+      <c r="N21" s="24">
+        <f t="shared" ref="N21:N24" si="17">F21/$F$25</f>
+        <v>0.21321494688907663</v>
+      </c>
+      <c r="O21" s="24">
+        <f t="shared" ref="O21:O24" si="18">G21/$G$25</f>
+        <v>0.20711909568619066</v>
+      </c>
+      <c r="P21" s="24">
+        <f t="shared" ref="P21:P24" si="19">H21/$H$25</f>
+        <v>0.27435207161858638</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.85723500000000008</v>
+      </c>
+      <c r="E22" s="1">
+        <v>150.56156250000001</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.27531875</v>
+      </c>
+      <c r="G22" s="1">
+        <v>31.3819625</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.32074999999999998</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" s="24">
+        <f t="shared" si="14"/>
+        <v>0.19975639464068209</v>
+      </c>
+      <c r="L22" s="24">
+        <f t="shared" si="15"/>
+        <v>0.18626326483552569</v>
+      </c>
+      <c r="M22" s="24">
+        <f t="shared" si="16"/>
+        <v>0.13403424835061736</v>
+      </c>
+      <c r="N22" s="24">
+        <f t="shared" si="17"/>
+        <v>0.20665741725657694</v>
+      </c>
+      <c r="O22" s="24">
+        <f t="shared" si="18"/>
+        <v>0.20494794579145828</v>
+      </c>
+      <c r="P22" s="24">
+        <f t="shared" si="19"/>
+        <v>0.20437421348583076</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="1">
+        <v>32.75</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.76771374999999997</v>
+      </c>
+      <c r="E23" s="1">
+        <v>242.95513750000003</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.28974375000000002</v>
+      </c>
+      <c r="G23" s="1">
+        <v>31.671812500000001</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.81810000000000005</v>
+      </c>
+      <c r="J23" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K23" s="24">
+        <f t="shared" si="14"/>
+        <v>0.31912302070645554</v>
+      </c>
+      <c r="L23" s="24">
+        <f t="shared" si="15"/>
+        <v>0.16681174886014283</v>
+      </c>
+      <c r="M23" s="24">
+        <f t="shared" si="16"/>
+        <v>0.21628567542086574</v>
+      </c>
+      <c r="N23" s="24">
+        <f t="shared" si="17"/>
+        <v>0.21748498800475929</v>
+      </c>
+      <c r="O23" s="24">
+        <f t="shared" si="18"/>
+        <v>0.20684088547257778</v>
+      </c>
+      <c r="P23" s="24">
+        <f t="shared" si="19"/>
+        <v>0.52127371489558283</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>28.375</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1.1402274999999999</v>
+      </c>
+      <c r="E24" s="1">
+        <v>398.72090000000003</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.15007087499999999</v>
+      </c>
+      <c r="G24" s="1">
+        <v>28.111774999999998</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="24">
+        <f t="shared" si="14"/>
+        <v>0.27649208282582216</v>
+      </c>
+      <c r="L24" s="24">
+        <f t="shared" si="15"/>
+        <v>0.24775294616441157</v>
+      </c>
+      <c r="M24" s="24">
+        <f t="shared" si="16"/>
+        <v>0.3549528528118302</v>
+      </c>
+      <c r="N24" s="24">
+        <f t="shared" si="17"/>
+        <v>0.11264492314066732</v>
+      </c>
+      <c r="O24" s="24">
+        <f t="shared" si="18"/>
+        <v>0.18359114853960046</v>
+      </c>
+      <c r="P24" s="24">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="25">
+        <f>SUM(C20:C24)</f>
+        <v>102.625</v>
+      </c>
+      <c r="D25" s="25">
+        <f t="shared" ref="D25:H25" si="20">SUM(D20:D24)</f>
+        <v>4.6022762500000001</v>
+      </c>
+      <c r="E25" s="25">
+        <f t="shared" si="20"/>
+        <v>1123.30665</v>
+      </c>
+      <c r="F25" s="25">
+        <f t="shared" si="20"/>
+        <v>1.3322471249999999</v>
+      </c>
+      <c r="G25" s="25">
+        <f t="shared" si="20"/>
+        <v>153.12162499999999</v>
+      </c>
+      <c r="H25" s="25">
+        <f t="shared" si="20"/>
+        <v>1.5694250000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B29720-46E5-4342-BBA4-B9C9D1D80DDF}">
   <dimension ref="A2:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3838,31 +4835,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="10" t="s">
         <v>16</v>
       </c>
       <c r="M2" s="1">
@@ -3891,15 +4888,15 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="11"/>
-      <c r="L3" s="15" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="22"/>
+      <c r="L3" s="11" t="s">
         <v>17</v>
       </c>
       <c r="M3" s="1">
@@ -3931,28 +4928,28 @@
       <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="2">
         <v>0.15</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="2">
         <v>-0.2</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="2">
         <v>0.15</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="2">
         <v>0.15</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="2">
         <v>-0.2</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="2">
         <v>0.15</v>
       </c>
     </row>
@@ -3960,7 +4957,7 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="18" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -3989,16 +4986,16 @@
       <c r="D6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="11">
         <v>3.25</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="9">
         <v>1.1628212500000001</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="11">
         <v>41.3352875</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="10">
         <v>0.28368749999999993</v>
       </c>
       <c r="I6" s="1">
@@ -4015,7 +5012,7 @@
       <c r="E7" s="1">
         <v>7.2</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>1.0776162499999999</v>
       </c>
       <c r="G7" s="1">
@@ -4027,7 +5024,7 @@
       <c r="I7" s="1">
         <v>9.4863999999999997</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="10">
         <v>0.91874999999999996</v>
       </c>
     </row>
@@ -4038,7 +5035,7 @@
       <c r="E8" s="1">
         <v>8.25</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>1.0680375000000002</v>
       </c>
       <c r="G8" s="1">
@@ -4061,7 +5058,7 @@
       <c r="E9" s="1">
         <v>9</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="8">
         <v>1.0519937500000001</v>
       </c>
       <c r="G9" s="1">
@@ -4070,7 +5067,7 @@
       <c r="H9" s="1">
         <v>0.24605874999999999</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="11">
         <v>9.5867374999999999</v>
       </c>
       <c r="J9" s="1">
@@ -4081,84 +5078,84 @@
       <c r="D10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="10">
         <v>9.875</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>1.07784375</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="10">
         <v>43.577583750000002</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="11">
         <v>0.19357875000000002</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="10">
         <v>7.9062000000000001</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
+    <row r="12" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="14" t="s">
+      <c r="L14" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="11"/>
-      <c r="L15" s="15" t="s">
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="22"/>
+      <c r="L15" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4166,24 +5163,24 @@
       <c r="B16" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="18" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -4209,7 +5206,7 @@
       <c r="D18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="17">
         <v>3.625</v>
       </c>
       <c r="F18" s="1">
@@ -4218,10 +5215,10 @@
       <c r="G18" s="1">
         <v>105.5400125</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="10">
         <v>0.36161624999999997</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="10">
         <v>15.109075000000001</v>
       </c>
       <c r="J18" s="1">
@@ -4232,10 +5229,10 @@
       <c r="D19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>17.375</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="10">
         <v>0.87214000000000003</v>
       </c>
       <c r="G19" s="1">
@@ -4255,13 +5252,13 @@
       <c r="D20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>25.25</v>
       </c>
       <c r="F20" s="1">
         <v>0.94584125000000008</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="11">
         <v>104.21896249999999</v>
       </c>
       <c r="H20" s="1">
@@ -4278,7 +5275,7 @@
       <c r="D21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="16">
         <v>26</v>
       </c>
       <c r="F21" s="1">
@@ -4290,10 +5287,10 @@
       <c r="H21" s="1">
         <v>0.20208625000000002</v>
       </c>
-      <c r="I21" s="15">
+      <c r="I21" s="11">
         <v>16.938724999999998</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="10">
         <v>0.63659999999999994</v>
       </c>
     </row>
@@ -4301,84 +5298,84 @@
       <c r="D22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="16">
         <v>26</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="11">
         <v>1.0771375000000001</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="10">
         <v>149.91706249999999</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="11">
         <v>0.18686049999999998</v>
       </c>
       <c r="I22" s="1">
         <v>15.222837500000001</v>
       </c>
-      <c r="J22" s="15">
+      <c r="J22" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D23" s="2"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="19"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="14"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="I26" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J26" s="7" t="s">
+      <c r="J26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L26" s="14" t="s">
+      <c r="L26" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="11"/>
-      <c r="L27" s="15" t="s">
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="22"/>
+      <c r="L27" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4386,24 +5383,24 @@
       <c r="B28" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="18" t="s">
         <v>23</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -4429,22 +5426,22 @@
       <c r="D30" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="11">
         <v>3.25</v>
       </c>
       <c r="F30" s="1">
         <v>1.06041125</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G30" s="11">
         <v>137.13126249999999</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="10">
         <v>0.33305875000000001</v>
       </c>
       <c r="I30" s="1">
         <v>30.2416625</v>
       </c>
-      <c r="J30" s="15">
+      <c r="J30" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4464,7 +5461,7 @@
       <c r="H31" s="1">
         <v>0.284055</v>
       </c>
-      <c r="I31" s="15">
+      <c r="I31" s="11">
         <v>31.714412500000002</v>
       </c>
       <c r="J31" s="1">
@@ -4498,10 +5495,10 @@
       <c r="D33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="10">
         <v>32.75</v>
       </c>
-      <c r="F33" s="14">
+      <c r="F33" s="10">
         <v>0.76771374999999997</v>
       </c>
       <c r="G33" s="1">
@@ -4513,7 +5510,7 @@
       <c r="I33" s="1">
         <v>31.671812500000001</v>
       </c>
-      <c r="J33" s="14">
+      <c r="J33" s="10">
         <v>0.81810000000000005</v>
       </c>
     </row>
@@ -4524,19 +5521,19 @@
       <c r="E34" s="1">
         <v>28.375</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F34" s="11">
         <v>1.1402274999999999</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G34" s="10">
         <v>398.72090000000003</v>
       </c>
-      <c r="H34" s="15">
+      <c r="H34" s="11">
         <v>0.15007087499999999</v>
       </c>
-      <c r="I34" s="14">
+      <c r="I34" s="10">
         <v>28.111774999999998</v>
       </c>
-      <c r="J34" s="15">
+      <c r="J34" s="11">
         <v>0</v>
       </c>
     </row>

</xml_diff>